<commit_message>
java codes are removed
</commit_message>
<xml_diff>
--- a/testng_project/src/test/resources/TestData/Amazon.xlsx
+++ b/testng_project/src/test/resources/TestData/Amazon.xlsx
@@ -540,7 +540,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
all codes are added
</commit_message>
<xml_diff>
--- a/testng_project/src/test/resources/TestData/Amazon.xlsx
+++ b/testng_project/src/test/resources/TestData/Amazon.xlsx
@@ -7,11 +7,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -81,6 +82,15 @@
   </si>
   <si>
     <t>testcase09</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -539,8 +549,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -661,4 +671,160 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.554688" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>